<commit_message>
Netzplan Wiederholung (Tabelle 3)
</commit_message>
<xml_diff>
--- a/Übungen/04_Netzplan_Wiederholung.xlsx
+++ b/Übungen/04_Netzplan_Wiederholung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="38">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">Endzeit →</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J</t>
   </si>
   <si>
     <t xml:space="preserve">Kritischer Pfad</t>
@@ -222,7 +225,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,7 +259,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFAFAFA"/>
       </patternFill>
     </fill>
     <fill>
@@ -273,12 +276,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAFA"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE8E8E8"/>
-        <bgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFAFAFA"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -335,6 +344,41 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -367,7 +411,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -444,7 +488,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,7 +508,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -520,20 +580,44 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -696,7 +780,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFAFAFA"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -807,13 +891,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>117000</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>68760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266760</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
@@ -823,7 +907,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1196640" y="8196840"/>
+          <a:off x="1196640" y="9009720"/>
           <a:ext cx="1769040" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -846,300 +930,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="810000" y="1629000"/>
-          <a:ext cx="540000" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25200">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2159280" y="1629000"/>
-          <a:ext cx="540360" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25200">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3508560" y="1629000"/>
-          <a:ext cx="540360" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25200">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>264600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1074240" y="2603880"/>
-          <a:ext cx="275760" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25200">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2159280" y="2603520"/>
-          <a:ext cx="276480" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25200">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1081080" y="1627200"/>
-          <a:ext cx="6480" cy="992160"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25200">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2430360" y="1626480"/>
-          <a:ext cx="6480" cy="992160"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25200">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1150,8 +940,8 @@
   </sheetPr>
   <dimension ref="A1:BS44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE17" activeCellId="0" sqref="AE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2156,27 +1946,54 @@
         <v>0</v>
       </c>
       <c r="B12" s="15"/>
-      <c r="C12" s="19"/>
+      <c r="C12" s="19" t="n">
+        <f aca="false">A12+A14</f>
+        <v>2</v>
+      </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-      <c r="G12" s="0"/>
-      <c r="H12" s="0"/>
+      <c r="F12" s="20" t="n">
+        <f aca="false">C12</f>
+        <v>2</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="19" t="n">
+        <f aca="false">F12+F14</f>
+        <v>8</v>
+      </c>
       <c r="I12" s="0"/>
       <c r="J12" s="0"/>
-      <c r="K12" s="0"/>
-      <c r="L12" s="0"/>
-      <c r="M12" s="0"/>
+      <c r="K12" s="20" t="n">
+        <f aca="false">H12</f>
+        <v>8</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="19" t="n">
+        <f aca="false">K12+K14</f>
+        <v>15</v>
+      </c>
       <c r="N12" s="0"/>
       <c r="O12" s="0"/>
-      <c r="P12" s="0"/>
-      <c r="Q12" s="0"/>
-      <c r="R12" s="0"/>
+      <c r="P12" s="20" t="n">
+        <f aca="false">M12</f>
+        <v>15</v>
+      </c>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="19" t="n">
+        <f aca="false">P12+P14</f>
+        <v>21</v>
+      </c>
       <c r="S12" s="0"/>
       <c r="T12" s="0"/>
-      <c r="U12" s="0"/>
-      <c r="V12" s="0"/>
-      <c r="W12" s="0"/>
+      <c r="U12" s="20" t="n">
+        <f aca="false">R12</f>
+        <v>21</v>
+      </c>
+      <c r="V12" s="4"/>
+      <c r="W12" s="19" t="n">
+        <f aca="false">U12+U14</f>
+        <v>27</v>
+      </c>
       <c r="X12" s="0"/>
       <c r="Y12" s="0"/>
       <c r="Z12" s="0"/>
@@ -2184,37 +2001,41 @@
       <c r="AB12" s="0"/>
       <c r="AC12" s="0"/>
       <c r="AD12" s="0"/>
-      <c r="AE12" s="0"/>
-      <c r="AF12" s="0"/>
-      <c r="AG12" s="0"/>
-      <c r="AH12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="0"/>
-      <c r="H13" s="0"/>
+      <c r="F13" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
-      <c r="K13" s="0"/>
-      <c r="L13" s="0"/>
-      <c r="M13" s="0"/>
+      <c r="K13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
       <c r="N13" s="0"/>
       <c r="O13" s="0"/>
-      <c r="P13" s="0"/>
-      <c r="Q13" s="0"/>
-      <c r="R13" s="0"/>
+      <c r="P13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
       <c r="S13" s="0"/>
       <c r="T13" s="0"/>
-      <c r="U13" s="0"/>
-      <c r="V13" s="0"/>
-      <c r="W13" s="0"/>
+      <c r="U13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
       <c r="X13" s="0"/>
       <c r="Y13" s="0"/>
       <c r="Z13" s="0"/>
@@ -2222,92 +2043,137 @@
       <c r="AB13" s="0"/>
       <c r="AC13" s="0"/>
       <c r="AD13" s="0"/>
-      <c r="AE13" s="0"/>
-      <c r="AF13" s="0"/>
-      <c r="AG13" s="0"/>
-      <c r="AH13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="n">
+      <c r="A14" s="22" t="n">
         <f aca="false">VLOOKUP(A13,$A$2:$H$10,8)</f>
         <v>2</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="0"/>
-      <c r="H14" s="0"/>
-      <c r="I14" s="0"/>
-      <c r="J14" s="0"/>
-      <c r="K14" s="0"/>
-      <c r="L14" s="0"/>
-      <c r="M14" s="0"/>
-      <c r="N14" s="0"/>
-      <c r="O14" s="0"/>
-      <c r="P14" s="0"/>
-      <c r="Q14" s="0"/>
-      <c r="R14" s="0"/>
-      <c r="S14" s="0"/>
-      <c r="T14" s="0"/>
-      <c r="U14" s="0"/>
-      <c r="V14" s="0"/>
-      <c r="W14" s="0"/>
-      <c r="X14" s="0"/>
-      <c r="Y14" s="0"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="22" t="n">
+        <f aca="false">VLOOKUP(F13,$A$2:$H$10,8)</f>
+        <v>6</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="22" t="n">
+        <f aca="false">VLOOKUP(K13,$A$2:$H$10,8)</f>
+        <v>7</v>
+      </c>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="22" t="n">
+        <f aca="false">VLOOKUP(P13,$A$2:$H$10,8)</f>
+        <v>6</v>
+      </c>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="22" t="n">
+        <f aca="false">VLOOKUP(U13,$A$2:$H$10,8)</f>
+        <v>6</v>
+      </c>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="26"/>
       <c r="Z14" s="0"/>
       <c r="AA14" s="0"/>
       <c r="AB14" s="0"/>
       <c r="AC14" s="0"/>
       <c r="AD14" s="0"/>
-      <c r="AE14" s="0"/>
-      <c r="AF14" s="0"/>
-      <c r="AG14" s="0"/>
-      <c r="AH14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23"/>
+      <c r="A15" s="27" t="n">
+        <f aca="false">C15-A14</f>
+        <v>0</v>
+      </c>
       <c r="B15" s="15"/>
-      <c r="C15" s="23"/>
+      <c r="C15" s="27" t="n">
+        <f aca="false">MIN(F15,F21)</f>
+        <v>2</v>
+      </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27" t="n">
+        <f aca="false">H15-F14</f>
+        <v>2</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="27" t="n">
+        <f aca="false">K15</f>
+        <v>8</v>
+      </c>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
-      <c r="K15" s="0"/>
-      <c r="L15" s="0"/>
-      <c r="M15" s="0"/>
+      <c r="K15" s="27" t="n">
+        <f aca="false">M15-K14</f>
+        <v>8</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="27" t="n">
+        <f aca="false">P15</f>
+        <v>15</v>
+      </c>
       <c r="N15" s="0"/>
       <c r="O15" s="0"/>
-      <c r="P15" s="0"/>
-      <c r="Q15" s="0"/>
-      <c r="R15" s="0"/>
+      <c r="P15" s="27" t="n">
+        <f aca="false">R15-P14</f>
+        <v>15</v>
+      </c>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="27" t="n">
+        <f aca="false">U15</f>
+        <v>21</v>
+      </c>
       <c r="S15" s="0"/>
       <c r="T15" s="0"/>
-      <c r="U15" s="0"/>
-      <c r="V15" s="0"/>
-      <c r="W15" s="0"/>
+      <c r="U15" s="27" t="n">
+        <f aca="false">W15-U14</f>
+        <v>21</v>
+      </c>
+      <c r="V15" s="4"/>
+      <c r="W15" s="27" t="n">
+        <f aca="false">Z18</f>
+        <v>27</v>
+      </c>
       <c r="X15" s="0"/>
-      <c r="Y15" s="0"/>
-      <c r="Z15" s="0"/>
-      <c r="AA15" s="0"/>
-      <c r="AB15" s="0"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="20" t="n">
+        <f aca="false">MAX(W12,M18)</f>
+        <v>27</v>
+      </c>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="19" t="n">
+        <f aca="false">Z15+Z17</f>
+        <v>31</v>
+      </c>
       <c r="AC15" s="0"/>
       <c r="AD15" s="0"/>
-      <c r="AE15" s="0"/>
-      <c r="AF15" s="0"/>
-      <c r="AG15" s="0"/>
-      <c r="AH15" s="0"/>
+      <c r="AE15" s="20" t="n">
+        <f aca="false">AB15</f>
+        <v>31</v>
+      </c>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="19" t="n">
+        <f aca="false">AE15+AE17</f>
+        <v>36</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
@@ -2327,23 +2193,26 @@
       <c r="V16" s="0"/>
       <c r="W16" s="0"/>
       <c r="X16" s="0"/>
-      <c r="Y16" s="0"/>
-      <c r="Z16" s="0"/>
-      <c r="AA16" s="0"/>
-      <c r="AB16" s="0"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA16" s="21"/>
+      <c r="AB16" s="21"/>
       <c r="AC16" s="0"/>
       <c r="AD16" s="0"/>
-      <c r="AE16" s="0"/>
-      <c r="AF16" s="0"/>
-      <c r="AG16" s="0"/>
-      <c r="AH16" s="0"/>
+      <c r="AE16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF16" s="21"/>
+      <c r="AG16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
@@ -2364,30 +2233,52 @@
       <c r="W17" s="0"/>
       <c r="X17" s="0"/>
       <c r="Y17" s="0"/>
-      <c r="Z17" s="0"/>
-      <c r="AA17" s="0"/>
-      <c r="AB17" s="0"/>
-      <c r="AC17" s="0"/>
-      <c r="AD17" s="0"/>
-      <c r="AE17" s="0"/>
-      <c r="AF17" s="0"/>
-      <c r="AG17" s="0"/>
-      <c r="AH17" s="0"/>
+      <c r="Z17" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA17" s="23" t="n">
+        <f aca="false">AB18-AB15</f>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="24"/>
+      <c r="AE17" s="22" t="n">
+        <f aca="false">VLOOKUP(AE16,$A$2:$H$10,8)</f>
+        <v>5</v>
+      </c>
+      <c r="AF17" s="23" t="n">
+        <f aca="false">AG18-AG15</f>
+        <v>0</v>
+      </c>
+      <c r="AG17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="0"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="20" t="n">
+        <f aca="false">C12</f>
+        <v>2</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="19" t="n">
+        <f aca="false">F18+F20</f>
+        <v>6</v>
+      </c>
       <c r="I18" s="0"/>
       <c r="J18" s="0"/>
-      <c r="K18" s="0"/>
-      <c r="L18" s="0"/>
-      <c r="M18" s="0"/>
+      <c r="K18" s="20" t="n">
+        <f aca="false">H18</f>
+        <v>6</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="19" t="n">
+        <f aca="false">K18+K20</f>
+        <v>15</v>
+      </c>
       <c r="N18" s="0"/>
       <c r="O18" s="0"/>
       <c r="P18" s="0"/>
@@ -2399,28 +2290,43 @@
       <c r="V18" s="0"/>
       <c r="W18" s="0"/>
       <c r="X18" s="0"/>
-      <c r="Y18" s="0"/>
-      <c r="Z18" s="0"/>
-      <c r="AA18" s="0"/>
-      <c r="AB18" s="0"/>
+      <c r="Y18" s="25"/>
+      <c r="Z18" s="27" t="n">
+        <f aca="false">AB18-Z17</f>
+        <v>27</v>
+      </c>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="27" t="n">
+        <f aca="false">AE18</f>
+        <v>31</v>
+      </c>
       <c r="AC18" s="0"/>
       <c r="AD18" s="0"/>
-      <c r="AE18" s="0"/>
-      <c r="AF18" s="0"/>
-      <c r="AG18" s="0"/>
-      <c r="AH18" s="0"/>
+      <c r="AE18" s="27" t="n">
+        <f aca="false">AG18-AE17</f>
+        <v>31</v>
+      </c>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="27" t="n">
+        <f aca="false">AG15</f>
+        <v>36</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="0"/>
       <c r="J19" s="0"/>
-      <c r="K19" s="0"/>
-      <c r="L19" s="0"/>
-      <c r="M19" s="0"/>
+      <c r="K19" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
       <c r="N19" s="0"/>
       <c r="O19" s="0"/>
       <c r="P19" s="0"/>
@@ -2432,7 +2338,7 @@
       <c r="V19" s="0"/>
       <c r="W19" s="0"/>
       <c r="X19" s="0"/>
-      <c r="Y19" s="0"/>
+      <c r="Y19" s="26"/>
       <c r="Z19" s="0"/>
       <c r="AA19" s="0"/>
       <c r="AB19" s="0"/>
@@ -2441,52 +2347,65 @@
       <c r="AE19" s="0"/>
       <c r="AF19" s="0"/>
       <c r="AG19" s="0"/>
-      <c r="AH19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
-      <c r="F20" s="0"/>
-      <c r="G20" s="0"/>
-      <c r="H20" s="0"/>
-      <c r="I20" s="0"/>
-      <c r="J20" s="0"/>
-      <c r="K20" s="0"/>
-      <c r="L20" s="0"/>
-      <c r="M20" s="0"/>
-      <c r="N20" s="0"/>
-      <c r="O20" s="0"/>
-      <c r="P20" s="0"/>
-      <c r="Q20" s="0"/>
-      <c r="R20" s="0"/>
-      <c r="S20" s="0"/>
-      <c r="T20" s="0"/>
-      <c r="U20" s="0"/>
-      <c r="V20" s="0"/>
-      <c r="W20" s="0"/>
-      <c r="X20" s="0"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="22" t="n">
+        <f aca="false">VLOOKUP(F19,$A$2:$H$10,8)</f>
+        <v>4</v>
+      </c>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="22" t="n">
+        <f aca="false">VLOOKUP(K19,$A$2:$H$10,8)</f>
+        <v>9</v>
+      </c>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
       <c r="Y20" s="0"/>
       <c r="Z20" s="0"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
-      <c r="AE20" s="0"/>
-      <c r="AF20" s="0"/>
-      <c r="AG20" s="0"/>
-      <c r="AH20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0"/>
       <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
-      <c r="H21" s="0"/>
+      <c r="F21" s="27" t="n">
+        <f aca="false">H21-F20</f>
+        <v>14</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="27" t="n">
+        <f aca="false">K21</f>
+        <v>18</v>
+      </c>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
-      <c r="K21" s="0"/>
-      <c r="L21" s="0"/>
-      <c r="M21" s="0"/>
+      <c r="K21" s="27" t="n">
+        <f aca="false">M21-K20</f>
+        <v>18</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="27" t="n">
+        <f aca="false">Z18</f>
+        <v>27</v>
+      </c>
       <c r="N21" s="0"/>
       <c r="O21" s="0"/>
       <c r="P21" s="0"/>
@@ -2504,43 +2423,6 @@
       <c r="AB21" s="0"/>
       <c r="AC21" s="0"/>
       <c r="AD21" s="0"/>
-      <c r="AE21" s="0"/>
-      <c r="AF21" s="0"/>
-      <c r="AG21" s="0"/>
-      <c r="AH21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="0"/>
-      <c r="E22" s="0"/>
-      <c r="F22" s="0"/>
-      <c r="G22" s="0"/>
-      <c r="H22" s="0"/>
-      <c r="I22" s="0"/>
-      <c r="J22" s="0"/>
-      <c r="K22" s="0"/>
-      <c r="L22" s="0"/>
-      <c r="M22" s="0"/>
-      <c r="N22" s="0"/>
-      <c r="O22" s="0"/>
-      <c r="P22" s="0"/>
-      <c r="Q22" s="0"/>
-      <c r="R22" s="0"/>
-      <c r="S22" s="0"/>
-      <c r="T22" s="0"/>
-      <c r="U22" s="0"/>
-      <c r="V22" s="0"/>
-      <c r="W22" s="0"/>
-      <c r="X22" s="0"/>
-      <c r="Y22" s="0"/>
-      <c r="Z22" s="0"/>
-      <c r="AA22" s="0"/>
-      <c r="AB22" s="0"/>
-      <c r="AC22" s="0"/>
-      <c r="AD22" s="0"/>
-      <c r="AE22" s="0"/>
-      <c r="AF22" s="0"/>
-      <c r="AG22" s="0"/>
-      <c r="AH22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15"/>
@@ -2617,135 +2499,143 @@
       <c r="C32" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="24" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="25" t="s">
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="24" t="s">
+      <c r="J34" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="25" t="s">
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="R34" s="24" t="s">
+      <c r="R34" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="S34" s="24"/>
-      <c r="T34" s="24"/>
-      <c r="U34" s="24"/>
-      <c r="V34" s="24"/>
-      <c r="W34" s="24"/>
-      <c r="X34" s="24"/>
-      <c r="Y34" s="24"/>
-      <c r="Z34" s="24"/>
-      <c r="AA34" s="24"/>
-      <c r="AB34" s="24"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="28"/>
+      <c r="X34" s="28"/>
+      <c r="Y34" s="28"/>
+      <c r="Z34" s="28"/>
+      <c r="AA34" s="28"/>
+      <c r="AB34" s="28"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B35" s="15"/>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26"/>
-      <c r="C37" s="26"/>
+      <c r="A37" s="30"/>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="26"/>
-      <c r="C38" s="26"/>
+      <c r="A38" s="30"/>
+      <c r="C38" s="30"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="26"/>
-      <c r="C39" s="26"/>
+      <c r="A39" s="30"/>
+      <c r="C39" s="30"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="26"/>
-      <c r="C40" s="26"/>
+      <c r="A40" s="30"/>
+      <c r="C40" s="30"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="26"/>
-      <c r="C41" s="26"/>
+      <c r="A41" s="30"/>
+      <c r="C41" s="30"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="26"/>
-      <c r="C42" s="26"/>
+      <c r="A42" s="30"/>
+      <c r="C42" s="30"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="26"/>
-      <c r="C43" s="26"/>
+      <c r="A43" s="30"/>
+      <c r="C43" s="30"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="A44" s="30"/>
+      <c r="C44" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="20">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="Z16:AB16"/>
+    <mergeCell ref="AE16:AG16"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="K19:M19"/>
     <mergeCell ref="D32:H32"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="D33:H33"/>
@@ -2761,16 +2651,21 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B14 G14 G20 L14 L20 Q14 AA16 AF16 V14">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:BS8 J8:AF9 AJ9:AK9 AX10:BS10 AO9:AR9 J10:AT10 J1:BS7 AW9:BS9">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>IF(OR(WEEKDAY(J$1,1)=7,WEEKDAY(J$1,1)=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:BS8 J8:AF9 AJ9:AK9 AX10:BS10 AO9:AR9 J10:AT10 J2:BS7 AW9:BS9">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2790,569 +2685,770 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R63"/>
+  <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE2" activeCellId="0" sqref="AE2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA18" activeCellId="0" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="27" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="31" width="3.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="28" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="32" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="31" t="n">
+      <c r="G2" s="39"/>
+      <c r="H2" s="35" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="s">
+      <c r="B3" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="35" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="35" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="C5" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="35" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="35" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="35" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="35" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="35" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="35" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="35" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="44"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="31" t="n">
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="n">
+        <f aca="false" t="array" ref="A16:A16">VLOOKUP(A15,$A$2:$H$15,8)</f>
+        <v>3</v>
+      </c>
+      <c r="B16" s="46"/>
+      <c r="C16" s="23"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="23" t="n">
+        <f aca="false" t="array" ref="F16:F16">VLOOKUP(F15,$A$2:$H$15,8)</f>
+        <v>4</v>
+      </c>
+      <c r="G16" s="46"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+      <c r="K16" s="23" t="n">
+        <f aca="false" t="array" ref="K16:K16">VLOOKUP(K15,$A$2:$H$15,8)</f>
+        <v>4</v>
+      </c>
+      <c r="L16" s="46"/>
+      <c r="M16" s="23"/>
+      <c r="P16" s="0"/>
+      <c r="Q16" s="0"/>
+      <c r="R16" s="0"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="0"/>
+      <c r="V16" s="0"/>
+      <c r="W16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="27"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="49"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="49"/>
+      <c r="P17" s="0"/>
+      <c r="Q17" s="0"/>
+      <c r="R17" s="0"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="44"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="47"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="U18" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="45"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="47"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="23" t="n">
+        <f aca="false" t="array" ref="U19:U19">VLOOKUP(U18,$A$2:$H$15,8)</f>
+        <v>4</v>
+      </c>
+      <c r="V19" s="46"/>
+      <c r="W19" s="23"/>
+      <c r="Y19" s="48"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="47"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="44"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="44"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="49"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="43"/>
+      <c r="AB20" s="44"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="51"/>
+      <c r="F21" s="21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31" t="s">
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="48"/>
+      <c r="Z21" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA21" s="21"/>
+      <c r="AB21" s="21"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="23" t="n">
+        <f aca="false" t="array" ref="F22:F22">VLOOKUP(F21,$A$2:$H$15,8)</f>
+        <v>8</v>
+      </c>
+      <c r="G22" s="46"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="0"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="23" t="n">
+        <f aca="false" t="array" ref="K22:K22">VLOOKUP(K21,$A$2:$H$15,8)</f>
+        <v>4</v>
+      </c>
+      <c r="L22" s="46"/>
+      <c r="M22" s="23"/>
+      <c r="P22" s="23" t="n">
+        <f aca="false" t="array" ref="P22:P22">VLOOKUP(P21,$A$2:$H$15,8)</f>
         <v>7</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="35" t="s">
+      <c r="Q22" s="46"/>
+      <c r="R22" s="23"/>
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="23" t="n">
+        <f aca="false" t="array" ref="Z22:Z22">VLOOKUP(Z21,$A$2:$H$15,8)</f>
+        <v>6</v>
+      </c>
+      <c r="AA22" s="46"/>
+      <c r="AB22" s="23"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="27"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="49"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="49"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="49"/>
+      <c r="Y23" s="48"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="43"/>
+      <c r="AB23" s="49"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J24" s="47"/>
+      <c r="Y24" s="48"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J25" s="47"/>
+      <c r="Y25" s="48"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="47"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="44"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="44"/>
+      <c r="Y26" s="48"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J27" s="51"/>
+      <c r="K27" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="45"/>
+      <c r="P27" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="45"/>
+      <c r="T27" s="45"/>
+      <c r="U27" s="45"/>
+      <c r="V27" s="45"/>
+      <c r="W27" s="45"/>
+      <c r="X27" s="45"/>
+      <c r="Y27" s="48"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K28" s="23" t="n">
+        <f aca="false" t="array" ref="K28:K28">VLOOKUP(K27,$A$2:$H$15,8)</f>
+        <v>8</v>
+      </c>
+      <c r="L28" s="46"/>
+      <c r="M28" s="23"/>
+      <c r="P28" s="23" t="n">
+        <f aca="false" t="array" ref="P28:P28">VLOOKUP(P27,$A$2:$H$15,8)</f>
+        <v>6</v>
+      </c>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="23"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K29" s="27"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="49"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="49"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="52"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="53"/>
+      <c r="L55" s="53"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="52"/>
+      <c r="B56" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="54"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="54"/>
+      <c r="I56" s="54"/>
+      <c r="J56" s="54"/>
+      <c r="K56" s="54"/>
+      <c r="L56" s="53"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="52"/>
+      <c r="B57" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="56"/>
+      <c r="H57" s="56"/>
+      <c r="I57" s="56"/>
+      <c r="J57" s="56"/>
+      <c r="K57" s="54"/>
+      <c r="L57" s="53"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="52"/>
+      <c r="B58" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="31" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
+      <c r="C58" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="54"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="54"/>
+      <c r="I58" s="54"/>
+      <c r="J58" s="54"/>
+      <c r="K58" s="54"/>
+      <c r="L58" s="53"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="52"/>
+      <c r="B59" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="54"/>
+      <c r="F59" s="54"/>
+      <c r="G59" s="54"/>
+      <c r="H59" s="54"/>
+      <c r="I59" s="54"/>
+      <c r="J59" s="54"/>
+      <c r="K59" s="54"/>
+      <c r="L59" s="53"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="52"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="54"/>
+      <c r="I60" s="54"/>
+      <c r="J60" s="54"/>
+      <c r="K60" s="54"/>
+      <c r="L60" s="53"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="52"/>
+      <c r="B61" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="60"/>
+      <c r="L61" s="53"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="52"/>
+      <c r="B62" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="60"/>
+      <c r="E62" s="60"/>
+      <c r="F62" s="60"/>
+      <c r="G62" s="60"/>
+      <c r="H62" s="60"/>
+      <c r="I62" s="60"/>
+      <c r="J62" s="60"/>
+      <c r="K62" s="60"/>
+      <c r="L62" s="53"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="52"/>
+      <c r="B63" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
+      <c r="F63" s="60"/>
+      <c r="G63" s="60"/>
+      <c r="H63" s="60"/>
+      <c r="I63" s="60"/>
+      <c r="J63" s="60"/>
+      <c r="K63" s="60"/>
+      <c r="L63" s="53"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="52"/>
+      <c r="B64" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="60"/>
+      <c r="E64" s="60"/>
+      <c r="F64" s="60"/>
+      <c r="G64" s="60"/>
+      <c r="H64" s="60"/>
+      <c r="I64" s="60"/>
+      <c r="J64" s="60"/>
+      <c r="K64" s="60"/>
+      <c r="L64" s="53"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="52"/>
+      <c r="B65" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="31" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="31" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39" t="n">
-        <f aca="false">A9+A11</f>
-        <v>6</v>
-      </c>
-      <c r="F9" s="18" t="n">
-        <f aca="false">C9</f>
-        <v>6</v>
-      </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39" t="n">
-        <f aca="false">F9+F11</f>
-        <v>13</v>
-      </c>
-      <c r="K9" s="18" t="n">
-        <f aca="false">MAX(H9,H15)</f>
-        <v>13</v>
-      </c>
-      <c r="L9" s="38"/>
-      <c r="M9" s="39" t="n">
-        <f aca="false">K9+K11</f>
+      <c r="C65" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="60"/>
+      <c r="E65" s="60"/>
+      <c r="F65" s="60"/>
+      <c r="G65" s="60"/>
+      <c r="H65" s="60"/>
+      <c r="I65" s="60"/>
+      <c r="J65" s="60"/>
+      <c r="K65" s="60"/>
+      <c r="L65" s="53"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="52"/>
+      <c r="B66" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" s="60"/>
+      <c r="E66" s="60"/>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="60"/>
+      <c r="I66" s="60"/>
+      <c r="J66" s="60"/>
+      <c r="K66" s="60"/>
+      <c r="L66" s="53"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="52"/>
+      <c r="B67" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="18" t="n">
-        <f aca="false">M9</f>
-        <v>18</v>
-      </c>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="39" t="n">
-        <f aca="false">P9+P11</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="F10" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="K10" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="P10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="n">
-        <f aca="false" t="array" ref="A11:A11">VLOOKUP(A10,$A$2:$H$10,8)</f>
-        <v>6</v>
-      </c>
-      <c r="B11" s="40" t="n">
-        <f aca="false">C12-C9</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="F11" s="22" t="n">
-        <f aca="false" t="array" ref="F11:F11">VLOOKUP(F10,$A$2:$H$10,8)</f>
-        <v>7</v>
-      </c>
-      <c r="G11" s="40" t="n">
-        <f aca="false">H12-H9</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="K11" s="22" t="n">
-        <f aca="false" t="array" ref="K11:K11">VLOOKUP(K10,$A$2:$H$10,8)</f>
-        <v>5</v>
-      </c>
-      <c r="L11" s="40" t="n">
-        <f aca="false">M12-M9</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="22"/>
-      <c r="P11" s="22" t="n">
-        <f aca="false" t="array" ref="P11:P11">VLOOKUP(P10,$A$2:$H$10,8)</f>
-        <v>9</v>
-      </c>
-      <c r="Q11" s="40" t="n">
-        <f aca="false">R12-R9</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="22"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="41" t="n">
-        <f aca="false">MIN(F12,F18)</f>
-        <v>6</v>
-      </c>
-      <c r="F12" s="23" t="n">
-        <f aca="false">H12-F11</f>
-        <v>6</v>
-      </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="41" t="n">
-        <f aca="false">K12</f>
-        <v>13</v>
-      </c>
-      <c r="K12" s="23" t="n">
-        <f aca="false">M12-K11</f>
-        <v>13</v>
-      </c>
-      <c r="L12" s="38"/>
-      <c r="M12" s="41" t="n">
-        <f aca="false">P12</f>
-        <v>18</v>
-      </c>
-      <c r="P12" s="23" t="n">
-        <f aca="false">R12-P11</f>
-        <v>18</v>
-      </c>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="41" t="n">
-        <f aca="false">R9</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="18" t="n">
-        <f aca="false">C9</f>
-        <v>6</v>
-      </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39" t="n">
-        <f aca="false">F15+F17</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="22" t="n">
-        <f aca="false" t="array" ref="F17:F17">VLOOKUP(F16,$A$2:$H$10,8)</f>
-        <v>4</v>
-      </c>
-      <c r="G17" s="40" t="n">
-        <f aca="false">H18-H15</f>
-        <v>3</v>
-      </c>
-      <c r="H17" s="22"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="23" t="n">
-        <f aca="false">H18-F17</f>
-        <v>9</v>
-      </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="41" t="n">
-        <f aca="false">K12</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="42"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="42"/>
-      <c r="B51" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="44"/>
-      <c r="K51" s="44"/>
-      <c r="L51" s="43"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="42"/>
-      <c r="B52" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="44"/>
-      <c r="L52" s="43"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="42"/>
-      <c r="B53" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="44"/>
-      <c r="L53" s="43"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="42"/>
-      <c r="B54" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="44"/>
-      <c r="J54" s="44"/>
-      <c r="K54" s="44"/>
-      <c r="L54" s="43"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="42"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44"/>
-      <c r="I55" s="44"/>
-      <c r="J55" s="44"/>
-      <c r="K55" s="44"/>
-      <c r="L55" s="43"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="42"/>
-      <c r="B56" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="50"/>
-      <c r="I56" s="50"/>
-      <c r="J56" s="50"/>
-      <c r="K56" s="50"/>
-      <c r="L56" s="43"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="42"/>
-      <c r="B57" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="50"/>
-      <c r="K57" s="50"/>
-      <c r="L57" s="43"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="42"/>
-      <c r="B58" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="50"/>
-      <c r="H58" s="50"/>
-      <c r="I58" s="50"/>
-      <c r="J58" s="50"/>
-      <c r="K58" s="50"/>
-      <c r="L58" s="43"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="42"/>
-      <c r="B59" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="50"/>
-      <c r="L59" s="43"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="42"/>
-      <c r="B60" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="50"/>
-      <c r="H60" s="50"/>
-      <c r="I60" s="50"/>
-      <c r="J60" s="50"/>
-      <c r="K60" s="50"/>
-      <c r="L60" s="43"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="42"/>
-      <c r="B61" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-      <c r="L61" s="43"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="42"/>
-      <c r="B62" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="43"/>
-      <c r="K62" s="43"/>
-      <c r="L62" s="43"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="42"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="43"/>
-      <c r="K63" s="43"/>
-      <c r="L63" s="43"/>
+      <c r="C67" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="53"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="53"/>
+      <c r="G67" s="53"/>
+      <c r="H67" s="53"/>
+      <c r="I67" s="53"/>
+      <c r="J67" s="53"/>
+      <c r="K67" s="53"/>
+      <c r="L67" s="53"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="52"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="53"/>
+      <c r="D68" s="53"/>
+      <c r="E68" s="53"/>
+      <c r="F68" s="53"/>
+      <c r="G68" s="53"/>
+      <c r="H68" s="53"/>
+      <c r="I68" s="53"/>
+      <c r="J68" s="53"/>
+      <c r="K68" s="53"/>
+      <c r="L68" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="20">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="F52:J52"/>
-    <mergeCell ref="C56:K56"/>
-    <mergeCell ref="C57:K57"/>
-    <mergeCell ref="C58:K58"/>
-    <mergeCell ref="C59:K59"/>
-    <mergeCell ref="C60:K60"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="Z21:AB21"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="F57:J57"/>
     <mergeCell ref="C61:K61"/>
+    <mergeCell ref="C62:K62"/>
+    <mergeCell ref="C63:K63"/>
+    <mergeCell ref="C64:K64"/>
+    <mergeCell ref="C65:K65"/>
+    <mergeCell ref="C66:K66"/>
   </mergeCells>
-  <conditionalFormatting sqref="C52:C53 B61">
+  <conditionalFormatting sqref="C57:C58 B66">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11 G11 G17 L11 Q11">
+  <conditionalFormatting sqref="B16 G16 G22 L16 L22 Q22 L28 Q28 V19 AA22">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>